<commit_message>
Add all sprint deliverables
</commit_message>
<xml_diff>
--- a/docs/4_sprint_deliverables/Phase I/ProductBackLog - 1.xlsx
+++ b/docs/4_sprint_deliverables/Phase I/ProductBackLog - 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jr_Kns/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jr_Kns/git/mms-lottery-kitchen-v2/docs/4_sprint_deliverables/Phase II/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>User Story</t>
   </si>
@@ -64,14 +64,166 @@
     <t>Search Function</t>
   </si>
   <si>
-    <t xml:space="preserve">[As] Tutor and Student
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">[I can] search each other with subject, location, cost, date and gender </t>
   </si>
   <si>
     <t>[so that] I can select the most matching and reduce matching time.</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>EPIC2</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>US2-1</t>
+  </si>
+  <si>
+    <t>EPIC3</t>
+  </si>
+  <si>
+    <t>US3-1</t>
+  </si>
+  <si>
+    <t>EPIC4</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>US4-1</t>
+  </si>
+  <si>
+    <t>EPIC5</t>
+  </si>
+  <si>
+    <t>Create Course</t>
+  </si>
+  <si>
+    <t>US5-1</t>
+  </si>
+  <si>
+    <t>Acceptance Criterion 1</t>
+  </si>
+  <si>
+    <t>Acceptance Criterion 2</t>
+  </si>
+  <si>
+    <t>[As] Guest</t>
+  </si>
+  <si>
+    <t>[Given] that user input a correct tags which exist in the system</t>
+  </si>
+  <si>
+    <t>[Given] that user input an incorrect tags which not exist in the system</t>
+  </si>
+  <si>
+    <t>[When] user sending a query tags to search engine</t>
+  </si>
+  <si>
+    <t>[Then] ensure the search results is correct.</t>
+  </si>
+  <si>
+    <t>[Then] ensure the system can acknowledge an error and notify user corectly.</t>
+  </si>
+  <si>
+    <t>[Given] that user want to use their username which not exist in the system (valid)</t>
+  </si>
+  <si>
+    <t>[When] user filling information in the registration process</t>
+  </si>
+  <si>
+    <t>[Then] Ensure that thier can use their username with no problems.</t>
+  </si>
+  <si>
+    <t>[Given] that user want to use their username which already exist in the system (invalid)</t>
+  </si>
+  <si>
+    <t>[I can] register as a tutor</t>
+  </si>
+  <si>
+    <t>[I can] register as a learner</t>
+  </si>
+  <si>
+    <t>[As] Tutor, Learner and Guest</t>
+  </si>
+  <si>
+    <t>[So that] I can making a tutor activities such as create offer and next time I come back I don't have to fill my information in a form again.</t>
+  </si>
+  <si>
+    <t>[I can] login in to my existing account</t>
+  </si>
+  <si>
+    <t>[So that] I can access to my personal information and making an activities such as booking and searching in the system more quickly.</t>
+  </si>
+  <si>
+    <t>[As] Learner</t>
+  </si>
+  <si>
+    <t>[I can] booking course offers which created by tutor</t>
+  </si>
+  <si>
+    <t>[So that] I can learn a course and tutor that I want to.</t>
+  </si>
+  <si>
+    <t>[Given] that user input a correct username and password</t>
+  </si>
+  <si>
+    <t>[When] user trying to login</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can regcognize and provide a correct information for user.</t>
+  </si>
+  <si>
+    <t>[Given] that user input an incorrect username or password</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can regcognize and notify user for their mistake.</t>
+  </si>
+  <si>
+    <t>[Given] that Learner already logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[When] trying to enter a course booking process</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can provide a booking process for user.</t>
+  </si>
+  <si>
+    <t>[Given] that Learner not logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can notify user to log in before start a booking process.</t>
+  </si>
+  <si>
+    <t>[As] Tutor</t>
+  </si>
+  <si>
+    <t>[I can] create a course offers which I want to teach</t>
+  </si>
+  <si>
+    <t>[So that]  I can advertise my offer into the system.</t>
+  </si>
+  <si>
+    <t>[Given] that Tutor already logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[When] trying to enter a course creating process</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can provide a creating process for user.</t>
+  </si>
+  <si>
+    <t>[Given] that Tutor not logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can notify user to log in before start a creating process.</t>
+  </si>
+  <si>
+    <t>[So that]  I can making a learner activities such as review tutor and next time I  come back I don't have to fill my information in a form again.</t>
   </si>
 </sst>
 </file>
@@ -175,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -185,6 +337,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -503,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:I19"/>
+  <dimension ref="D7:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H12"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -514,17 +672,19 @@
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="52" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.6640625" customWidth="1"/>
+    <col min="8" max="8" width="56.83203125" customWidth="1"/>
+    <col min="9" max="9" width="62.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11" ht="21" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:11" ht="30" x14ac:dyDescent="0.2">
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
@@ -537,113 +697,471 @@
       <c r="G9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="4:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="D10" s="3" t="s">
+    <row r="10" spans="4:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="8">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="8">
+        <v>20</v>
+      </c>
+      <c r="K13" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="8">
+        <v>10</v>
+      </c>
+      <c r="K16" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="4:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="8">
+        <v>17</v>
+      </c>
+      <c r="K19" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="E22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="8">
+        <v>20</v>
+      </c>
+      <c r="K22" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="8">
+        <v>15</v>
+      </c>
+      <c r="K25" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
+  <mergeCells count="18">
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="K25:K27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ADD Redux and Change some Structure and Fix conflict
</commit_message>
<xml_diff>
--- a/docs/4_sprint_deliverables/Phase I/ProductBackLog - 1.xlsx
+++ b/docs/4_sprint_deliverables/Phase I/ProductBackLog - 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jr_Kns/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jr_Kns/git/mms-lottery-kitchen-v2/docs/4_sprint_deliverables/Phase II/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>User Story</t>
   </si>
@@ -64,14 +64,166 @@
     <t>Search Function</t>
   </si>
   <si>
-    <t xml:space="preserve">[As] Tutor and Student
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">[I can] search each other with subject, location, cost, date and gender </t>
   </si>
   <si>
     <t>[so that] I can select the most matching and reduce matching time.</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>EPIC2</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>US2-1</t>
+  </si>
+  <si>
+    <t>EPIC3</t>
+  </si>
+  <si>
+    <t>US3-1</t>
+  </si>
+  <si>
+    <t>EPIC4</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>US4-1</t>
+  </si>
+  <si>
+    <t>EPIC5</t>
+  </si>
+  <si>
+    <t>Create Course</t>
+  </si>
+  <si>
+    <t>US5-1</t>
+  </si>
+  <si>
+    <t>Acceptance Criterion 1</t>
+  </si>
+  <si>
+    <t>Acceptance Criterion 2</t>
+  </si>
+  <si>
+    <t>[As] Guest</t>
+  </si>
+  <si>
+    <t>[Given] that user input a correct tags which exist in the system</t>
+  </si>
+  <si>
+    <t>[Given] that user input an incorrect tags which not exist in the system</t>
+  </si>
+  <si>
+    <t>[When] user sending a query tags to search engine</t>
+  </si>
+  <si>
+    <t>[Then] ensure the search results is correct.</t>
+  </si>
+  <si>
+    <t>[Then] ensure the system can acknowledge an error and notify user corectly.</t>
+  </si>
+  <si>
+    <t>[Given] that user want to use their username which not exist in the system (valid)</t>
+  </si>
+  <si>
+    <t>[When] user filling information in the registration process</t>
+  </si>
+  <si>
+    <t>[Then] Ensure that thier can use their username with no problems.</t>
+  </si>
+  <si>
+    <t>[Given] that user want to use their username which already exist in the system (invalid)</t>
+  </si>
+  <si>
+    <t>[I can] register as a tutor</t>
+  </si>
+  <si>
+    <t>[I can] register as a learner</t>
+  </si>
+  <si>
+    <t>[As] Tutor, Learner and Guest</t>
+  </si>
+  <si>
+    <t>[So that] I can making a tutor activities such as create offer and next time I come back I don't have to fill my information in a form again.</t>
+  </si>
+  <si>
+    <t>[I can] login in to my existing account</t>
+  </si>
+  <si>
+    <t>[So that] I can access to my personal information and making an activities such as booking and searching in the system more quickly.</t>
+  </si>
+  <si>
+    <t>[As] Learner</t>
+  </si>
+  <si>
+    <t>[I can] booking course offers which created by tutor</t>
+  </si>
+  <si>
+    <t>[So that] I can learn a course and tutor that I want to.</t>
+  </si>
+  <si>
+    <t>[Given] that user input a correct username and password</t>
+  </si>
+  <si>
+    <t>[When] user trying to login</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can regcognize and provide a correct information for user.</t>
+  </si>
+  <si>
+    <t>[Given] that user input an incorrect username or password</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can regcognize and notify user for their mistake.</t>
+  </si>
+  <si>
+    <t>[Given] that Learner already logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[When] trying to enter a course booking process</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can provide a booking process for user.</t>
+  </si>
+  <si>
+    <t>[Given] that Learner not logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can notify user to log in before start a booking process.</t>
+  </si>
+  <si>
+    <t>[As] Tutor</t>
+  </si>
+  <si>
+    <t>[I can] create a course offers which I want to teach</t>
+  </si>
+  <si>
+    <t>[So that]  I can advertise my offer into the system.</t>
+  </si>
+  <si>
+    <t>[Given] that Tutor already logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[When] trying to enter a course creating process</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can provide a creating process for user.</t>
+  </si>
+  <si>
+    <t>[Given] that Tutor not logged into their account  (valid type account)</t>
+  </si>
+  <si>
+    <t>[Then] Ensure the system can notify user to log in before start a creating process.</t>
+  </si>
+  <si>
+    <t>[So that]  I can making a learner activities such as review tutor and next time I  come back I don't have to fill my information in a form again.</t>
   </si>
 </sst>
 </file>
@@ -175,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -185,6 +337,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -503,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:I19"/>
+  <dimension ref="D7:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H12"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -514,17 +672,19 @@
     <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="52" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.6640625" customWidth="1"/>
+    <col min="8" max="8" width="56.83203125" customWidth="1"/>
+    <col min="9" max="9" width="62.1640625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11" ht="21" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="4:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="4:11" ht="30" x14ac:dyDescent="0.2">
       <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
@@ -537,113 +697,471 @@
       <c r="G9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="4:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="D10" s="3" t="s">
+    <row r="10" spans="4:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="8">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="8">
+        <v>20</v>
+      </c>
+      <c r="K13" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="8">
+        <v>10</v>
+      </c>
+      <c r="K16" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="4:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="8">
+        <v>17</v>
+      </c>
+      <c r="K19" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="4:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="E22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="8">
+        <v>20</v>
+      </c>
+      <c r="K22" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="8">
+        <v>15</v>
+      </c>
+      <c r="K25" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="I10:I12"/>
+  <mergeCells count="18">
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="K25:K27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>